<commit_message>
finished script to generate summary stats for injected bugs
</commit_message>
<xml_diff>
--- a/Summary Stats.xlsx
+++ b/Summary Stats.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7419F67-07BE-436C-9C34-C6A145DBECBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D70BB1E-ECF8-4636-9C15-908CCB62865D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Codebase Stats</t>
   </si>
@@ -32,6 +32,51 @@
   </si>
   <si>
     <t># of 'valid/readable' lines in codebase</t>
+  </si>
+  <si>
+    <t>Injected Bugs Stats</t>
+  </si>
+  <si>
+    <t>Number of unique bug id's</t>
+  </si>
+  <si>
+    <t>Total number of alerts flagged in comments</t>
+  </si>
+  <si>
+    <t>Number of alerts associated with each CERT Code:</t>
+  </si>
+  <si>
+    <t>MEM35-C</t>
+  </si>
+  <si>
+    <t>ARR30-C</t>
+  </si>
+  <si>
+    <t>INT31-C</t>
+  </si>
+  <si>
+    <t>EXP34-C</t>
+  </si>
+  <si>
+    <t>EXP33-C</t>
+  </si>
+  <si>
+    <t>MSC21-C</t>
+  </si>
+  <si>
+    <t>MEM10-C</t>
+  </si>
+  <si>
+    <t>EXP08-C</t>
+  </si>
+  <si>
+    <t>MEM00-C</t>
+  </si>
+  <si>
+    <t>MEM01-C</t>
+  </si>
+  <si>
+    <t>MEM30-C</t>
   </si>
 </sst>
 </file>
@@ -358,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -398,6 +443,120 @@
         <v>24228350</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
started cataloging sql bugs
</commit_message>
<xml_diff>
--- a/Summary Stats.xlsx
+++ b/Summary Stats.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D70BB1E-ECF8-4636-9C15-908CCB62865D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD835ADB-24C5-4021-ABEC-5A50138B67AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Codebase Stats</t>
   </si>
@@ -46,37 +46,97 @@
     <t>Number of alerts associated with each CERT Code:</t>
   </si>
   <si>
-    <t>MEM35-C</t>
-  </si>
-  <si>
-    <t>ARR30-C</t>
-  </si>
-  <si>
-    <t>INT31-C</t>
-  </si>
-  <si>
-    <t>EXP34-C</t>
-  </si>
-  <si>
-    <t>EXP33-C</t>
-  </si>
-  <si>
-    <t>MSC21-C</t>
-  </si>
-  <si>
-    <t>MEM10-C</t>
-  </si>
-  <si>
-    <t>EXP08-C</t>
-  </si>
-  <si>
-    <t>MEM00-C</t>
-  </si>
-  <si>
-    <t>MEM01-C</t>
-  </si>
-  <si>
-    <t>MEM30-C</t>
+    <t>CWE-126</t>
+  </si>
+  <si>
+    <t>CWE-823</t>
+  </si>
+  <si>
+    <t>CWE-196</t>
+  </si>
+  <si>
+    <t>CWE-754</t>
+  </si>
+  <si>
+    <t>CWE-824</t>
+  </si>
+  <si>
+    <t>CWE-457</t>
+  </si>
+  <si>
+    <t>CWE-416</t>
+  </si>
+  <si>
+    <t>CWE-119</t>
+  </si>
+  <si>
+    <t>CWE-835</t>
+  </si>
+  <si>
+    <t>CWE-822</t>
+  </si>
+  <si>
+    <t>CWE-125</t>
+  </si>
+  <si>
+    <t>CWE-469</t>
+  </si>
+  <si>
+    <t>CWE-415</t>
+  </si>
+  <si>
+    <t>CWE-476</t>
+  </si>
+  <si>
+    <t>CWE-120</t>
+  </si>
+  <si>
+    <t>CWE-834</t>
+  </si>
+  <si>
+    <t>CWE-787</t>
+  </si>
+  <si>
+    <t>CWE-191</t>
+  </si>
+  <si>
+    <t>CWE-788</t>
+  </si>
+  <si>
+    <t>CWE-628</t>
+  </si>
+  <si>
+    <t>CWE-131</t>
+  </si>
+  <si>
+    <t>CWE-170</t>
+  </si>
+  <si>
+    <t>CWE-129</t>
+  </si>
+  <si>
+    <t>CWE-460</t>
+  </si>
+  <si>
+    <t>CWE-825</t>
+  </si>
+  <si>
+    <t>CWE-121</t>
+  </si>
+  <si>
+    <t>CWE-190</t>
+  </si>
+  <si>
+    <t>CWE-789</t>
+  </si>
+  <si>
+    <t>CWE-248</t>
+  </si>
+  <si>
+    <t>CWE-127</t>
+  </si>
+  <si>
+    <t>CWE-124</t>
   </si>
 </sst>
 </file>
@@ -403,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -482,7 +542,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -495,18 +555,18 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -514,7 +574,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -522,7 +582,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -530,7 +590,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -538,7 +598,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -546,7 +606,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -554,7 +614,175 @@
         <v>18</v>
       </c>
       <c r="B20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
         <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>